<commit_message>
Updating size of errorlogging.fpdsstage1
</commit_message>
<xml_diff>
--- a/ImportAids/FPDSstage1updateTool.xlsx
+++ b/ImportAids/FPDSstage1updateTool.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\Greg\Repositories\Lookup-Tables\ImportAids\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{3BE36238-3FD1-42DB-A39B-E4796AF3D457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F6C3C7E-4947-43AE-B40A-C8CC27E2C4DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ErrorLogging.FPDSstage1.Table" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="300">
   <si>
     <t>SET ANSI_NULLS ON</t>
   </si>
@@ -901,25 +914,31 @@
     <t>[recipient_parent_uei] [varchar](255) NULL,</t>
   </si>
   <si>
-    <t>[prime_award_base_transaction_description] [varchar](4008) NULL</t>
-  </si>
-  <si>
     <t>) ON [PRIMARY]</t>
   </si>
   <si>
-    <t>ALTER TABLE [ErrorLogging].[FPDSstage1] ADD  CONSTRAINT [DF__FPDSbetaV__CSISm__6FAB3F2B]  DEFAULT (getdate()) FOR [CSISmodifiedDate]</t>
-  </si>
-  <si>
-    <t>ALTER TABLE [ErrorLogging].[FPDSstage1] ADD  CONSTRAINT [DF__FPDSbetaV__CSISc__709F6364]  DEFAULT (getdate()) FOR [CSIScreatedDate]</t>
-  </si>
-  <si>
     <t/>
+  </si>
+  <si>
+    <t>[prime_award_base_transaction_description] [varchar](4008) NULL,</t>
+  </si>
+  <si>
+    <t>[obligated_amount_funded_by_IIJA_supplementals_for_overall_award] [varchar](255) NULL,</t>
+  </si>
+  <si>
+    <t>[outlayed_amount_funded_by_IIJA_supplementals_for_overall_award] [varchar](255) NULL,</t>
+  </si>
+  <si>
+    <t>[recipient_name_raw] [varchar](255) NULL,</t>
+  </si>
+  <si>
+    <t>[recipient_parent_name_raw] [varchar](255) NULL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1753,11 +1772,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G301"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G7:G19"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1805,7 +1824,7 @@
         <v/>
       </c>
       <c r="G6" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2013,7 +2032,7 @@
         <v/>
       </c>
       <c r="G19" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
@@ -5593,40 +5612,72 @@
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B295" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="C295" t="str">
         <f t="shared" si="8"/>
-        <v>400</v>
+        <v>008</v>
       </c>
       <c r="D295" t="str">
         <f t="shared" si="9"/>
-        <v>[prime_award_base_transaction_description] [varchar](4008) NULL</v>
+        <v>[prime_award_base_transaction_description] [varchar](4008) NULL,</v>
       </c>
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A296" t="s">
-        <v>294</v>
+      <c r="B296" t="s">
+        <v>296</v>
+      </c>
+      <c r="C296" t="str">
+        <f t="shared" ref="C296:C299" si="10">LEFT(RIGHT(B296,10),3)</f>
+        <v>255</v>
+      </c>
+      <c r="D296" t="str">
+        <f t="shared" ref="D296:D299" si="11">IF(C296&lt;&gt;"255",B296,"")</f>
+        <v/>
       </c>
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A297" t="s">
-        <v>1</v>
+      <c r="B297" t="s">
+        <v>297</v>
+      </c>
+      <c r="C297" t="str">
+        <f t="shared" si="10"/>
+        <v>255</v>
+      </c>
+      <c r="D297" t="str">
+        <f t="shared" si="11"/>
+        <v/>
       </c>
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A298" t="s">
-        <v>295</v>
+      <c r="B298" t="s">
+        <v>298</v>
+      </c>
+      <c r="C298" t="str">
+        <f t="shared" si="10"/>
+        <v>255</v>
+      </c>
+      <c r="D298" t="str">
+        <f t="shared" si="11"/>
+        <v/>
       </c>
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A299" t="s">
-        <v>1</v>
+      <c r="B299" t="s">
+        <v>299</v>
+      </c>
+      <c r="C299" t="str">
+        <f t="shared" si="10"/>
+        <v>(25</v>
+      </c>
+      <c r="D299" t="str">
+        <f t="shared" si="11"/>
+        <v>[recipient_parent_name_raw] [varchar](255) NULL</v>
       </c>
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Transaction description 6166   characters
</commit_message>
<xml_diff>
--- a/ImportAids/FPDSstage1updateTool.xlsx
+++ b/ImportAids/FPDSstage1updateTool.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\Greg\Repositories\Lookup-Tables\ImportAids\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4305274D-D5A4-4CAC-8793-E199442660A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0824DB8C-B2A0-4DFB-9737-9188630628ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1080" uniqueCount="668">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1080" uniqueCount="669">
   <si>
     <t>SET ANSI_NULLS ON</t>
   </si>
@@ -2042,6 +2042,9 @@
   </si>
   <si>
     <t>[funding_opportunity_goals_text] [varchar](2000) NULL,</t>
+  </si>
+  <si>
+    <t>[transaction_description] [varchar](6500) NULL,</t>
   </si>
 </sst>
 </file>
@@ -12090,7 +12093,7 @@
   <dimension ref="A1:N312"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B79" workbookViewId="0">
-      <selection activeCell="B93" sqref="B93"/>
+      <selection activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15176,7 +15179,7 @@
     </row>
     <row r="95" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>584</v>
+        <v>668</v>
       </c>
       <c r="C95" t="str">
         <f t="shared" si="8"/>
@@ -15188,11 +15191,11 @@
       </c>
       <c r="E95" t="str">
         <f t="shared" si="10"/>
-        <v>4008</v>
+        <v>6500</v>
       </c>
       <c r="F95" t="str">
         <f t="shared" si="9"/>
-        <v>[transaction_description] [varchar](4008) NULL,</v>
+        <v>[transaction_description] [varchar](6500) NULL,</v>
       </c>
       <c r="G95">
         <f t="shared" si="7"/>

</xml_diff>